<commit_message>
Checked that all examples are running
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_noclustering.xlsx
+++ b/ConfigFiles/Config_noclustering.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="2160" windowHeight="1185"/>
@@ -453,9 +453,6 @@
     <t>Database/Load_RealTime/##/1h/2015.csv</t>
   </si>
   <si>
-    <t>Database/PowerPlants/##/2015_sto.csv</t>
-  </si>
-  <si>
     <t>Database/AvailabilityFactors/##/1h/2015.csv</t>
   </si>
   <si>
@@ -481,6 +478,9 @@
   </si>
   <si>
     <t>Simulations/simulation_Noclustering</t>
+  </si>
+  <si>
+    <t>Database/PowerPlants/##/2015.csv</t>
   </si>
 </sst>
 </file>
@@ -969,8 +969,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,7 +1074,7 @@
         <v>37</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D18" s="14"/>
       <c r="H18" s="1" t="s">
@@ -1326,7 +1326,7 @@
         <v>37</v>
       </c>
       <c r="C64" s="24" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="D64" s="22" t="s">
         <v>92</v>
@@ -1343,7 +1343,7 @@
         <v>37</v>
       </c>
       <c r="C65" s="24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D65" s="22" t="s">
         <v>92</v>
@@ -1378,7 +1378,7 @@
         <v>37</v>
       </c>
       <c r="C67" s="24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D67" s="22" t="s">
         <v>92</v>
@@ -1395,7 +1395,7 @@
         <v>37</v>
       </c>
       <c r="C68" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D68" s="22" t="s">
         <v>92</v>
@@ -1412,7 +1412,7 @@
         <v>37</v>
       </c>
       <c r="C69" s="24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D69" s="22" t="s">
         <v>92</v>
@@ -1546,7 +1546,7 @@
         <v>37</v>
       </c>
       <c r="C76" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D76" s="22" t="s">
         <v>92</v>
@@ -1636,7 +1636,7 @@
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="30"/>
       <c r="B89" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C89" s="4" t="b">
         <v>1</v>
@@ -1717,7 +1717,7 @@
         <v>1</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F94" s="5" t="b">
         <v>1</v>
@@ -2177,7 +2177,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C2" t="s">
         <v>61</v>

</xml_diff>